<commit_message>
Auto push full batch
</commit_message>
<xml_diff>
--- a/deal_links.xlsx
+++ b/deal_links.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,15 +476,20 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>ROI שכירות</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>מאושר</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>סיכום</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>צפה</t>
         </is>
@@ -531,15 +536,20 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
           <t>כן</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>רווחי</t>
         </is>
       </c>
-      <c r="K2">
+      <c r="L2">
         <f>HYPERLINK("https://friesiancapital.github.io/Analysis-/deal001.html", "צפה")</f>
         <v/>
       </c>
@@ -585,15 +595,20 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>לא</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>סיכון גבוה</t>
-        </is>
-      </c>
-      <c r="K3">
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>גבולי/לא משתלם</t>
+        </is>
+      </c>
+      <c r="L3">
         <f>HYPERLINK("https://friesiancapital.github.io/Analysis-/deal002.html", "צפה")</f>
         <v/>
       </c>
@@ -639,15 +654,20 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
           <t>לא</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>סיכון גבוה</t>
-        </is>
-      </c>
-      <c r="K4">
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>גבולי/לא משתלם</t>
+        </is>
+      </c>
+      <c r="L4">
         <f>HYPERLINK("https://friesiancapital.github.io/Analysis-/deal003.html", "צפה")</f>
         <v/>
       </c>

</xml_diff>